<commit_message>
added functionality to interpolate daily spot rates on the yield curve using a cubic spline method and store into a database. This will be used to calculate and validate zspread figures
</commit_message>
<xml_diff>
--- a/GBP Bonds/Master List of Bonds/Service Companies -disc.xlsx
+++ b/GBP Bonds/Master List of Bonds/Service Companies -disc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renea\OneDrive\Documents\University of Bath\13. Dissertation\Data\GBP Bonds\Master List of Bonds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257C750A-91B7-45CC-B640-927E168A5AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66B041E-078A-4253-B1FF-6BF54279C802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8338" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8330" uniqueCount="443">
   <si>
     <t>Issuer</t>
   </si>
@@ -626,9 +626,6 @@
   </si>
   <si>
     <t>GB0003806725</t>
-  </si>
-  <si>
-    <t>--</t>
   </si>
   <si>
     <t>XS0996777834</t>
@@ -1737,7 +1734,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11525,9 +11524,6 @@
       <c r="L65" t="s">
         <v>57</v>
       </c>
-      <c r="M65" t="s">
-        <v>202</v>
-      </c>
       <c r="N65" t="s">
         <v>19</v>
       </c>
@@ -11660,7 +11656,7 @@
         <v>41606</v>
       </c>
       <c r="F66" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H66" t="s">
         <v>53</v>
@@ -11812,7 +11808,7 @@
         <v>41858</v>
       </c>
       <c r="F67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H67" t="s">
         <v>53</v>
@@ -11949,10 +11945,10 @@
     </row>
     <row r="68" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>204</v>
+      </c>
+      <c r="B68" t="s">
         <v>205</v>
-      </c>
-      <c r="B68" t="s">
-        <v>206</v>
       </c>
       <c r="C68" s="1">
         <v>10.75</v>
@@ -11964,7 +11960,7 @@
         <v>32574</v>
       </c>
       <c r="F68" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H68" t="s">
         <v>53</v>
@@ -12101,10 +12097,10 @@
     </row>
     <row r="69" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>207</v>
+      </c>
+      <c r="B69" t="s">
         <v>208</v>
-      </c>
-      <c r="B69" t="s">
-        <v>209</v>
       </c>
       <c r="C69" s="1">
         <v>8.75</v>
@@ -12116,7 +12112,7 @@
         <v>36831</v>
       </c>
       <c r="F69" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H69" t="s">
         <v>53</v>
@@ -12137,10 +12133,10 @@
         <v>149911425.22571999</v>
       </c>
       <c r="N69" t="s">
+        <v>210</v>
+      </c>
+      <c r="O69" t="s">
         <v>211</v>
-      </c>
-      <c r="O69" t="s">
-        <v>212</v>
       </c>
       <c r="P69" t="s">
         <v>59</v>
@@ -12253,10 +12249,10 @@
     </row>
     <row r="70" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" t="s">
         <v>213</v>
-      </c>
-      <c r="B70" t="s">
-        <v>214</v>
       </c>
       <c r="C70" s="1">
         <v>6</v>
@@ -12268,7 +12264,7 @@
         <v>41449</v>
       </c>
       <c r="F70" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H70" t="s">
         <v>53</v>
@@ -12405,10 +12401,10 @@
     </row>
     <row r="71" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>215</v>
+      </c>
+      <c r="B71" t="s">
         <v>216</v>
-      </c>
-      <c r="B71" t="s">
-        <v>217</v>
       </c>
       <c r="C71" s="1">
         <v>3.2879999999999998</v>
@@ -12420,7 +12416,7 @@
         <v>44587</v>
       </c>
       <c r="F71" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H71" t="s">
         <v>53</v>
@@ -12557,10 +12553,10 @@
     </row>
     <row r="72" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>218</v>
+      </c>
+      <c r="B72" t="s">
         <v>219</v>
-      </c>
-      <c r="B72" t="s">
-        <v>220</v>
       </c>
       <c r="C72" s="1">
         <v>8</v>
@@ -12572,7 +12568,7 @@
         <v>44127</v>
       </c>
       <c r="F72" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H72" t="s">
         <v>53</v>
@@ -12709,10 +12705,10 @@
     </row>
     <row r="73" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>221</v>
+      </c>
+      <c r="B73" t="s">
         <v>222</v>
-      </c>
-      <c r="B73" t="s">
-        <v>223</v>
       </c>
       <c r="C73" s="1">
         <v>6</v>
@@ -12724,7 +12720,7 @@
         <v>40156</v>
       </c>
       <c r="F73" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H73" t="s">
         <v>53</v>
@@ -12861,10 +12857,10 @@
     </row>
     <row r="74" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>221</v>
+      </c>
+      <c r="B74" t="s">
         <v>222</v>
-      </c>
-      <c r="B74" t="s">
-        <v>223</v>
       </c>
       <c r="C74" s="1">
         <v>3.875</v>
@@ -12876,7 +12872,7 @@
         <v>41241</v>
       </c>
       <c r="F74" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H74" t="s">
         <v>53</v>
@@ -13013,10 +13009,10 @@
     </row>
     <row r="75" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>225</v>
+      </c>
+      <c r="B75" t="s">
         <v>226</v>
-      </c>
-      <c r="B75" t="s">
-        <v>227</v>
       </c>
       <c r="C75" s="1">
         <v>11.25</v>
@@ -13028,7 +13024,7 @@
         <v>32519</v>
       </c>
       <c r="F75" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H75" t="s">
         <v>53</v>
@@ -13052,7 +13048,7 @@
         <v>74</v>
       </c>
       <c r="O75" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P75" t="s">
         <v>59</v>
@@ -13165,10 +13161,10 @@
     </row>
     <row r="76" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>225</v>
+      </c>
+      <c r="B76" t="s">
         <v>226</v>
-      </c>
-      <c r="B76" t="s">
-        <v>227</v>
       </c>
       <c r="C76" s="1">
         <v>5.625</v>
@@ -13180,7 +13176,7 @@
         <v>36221</v>
       </c>
       <c r="F76" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H76" t="s">
         <v>53</v>
@@ -13204,7 +13200,7 @@
         <v>19</v>
       </c>
       <c r="O76" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P76" t="s">
         <v>59</v>
@@ -13317,10 +13313,10 @@
     </row>
     <row r="77" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>225</v>
+      </c>
+      <c r="B77" t="s">
         <v>226</v>
-      </c>
-      <c r="B77" t="s">
-        <v>227</v>
       </c>
       <c r="C77" s="1">
         <v>5.375</v>
@@ -13332,7 +13328,7 @@
         <v>38644</v>
       </c>
       <c r="F77" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H77" t="s">
         <v>53</v>
@@ -13356,7 +13352,7 @@
         <v>19</v>
       </c>
       <c r="O77" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P77" t="s">
         <v>59</v>
@@ -13469,10 +13465,10 @@
     </row>
     <row r="78" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>225</v>
+      </c>
+      <c r="B78" t="s">
         <v>226</v>
-      </c>
-      <c r="B78" t="s">
-        <v>227</v>
       </c>
       <c r="D78" s="2">
         <v>109939</v>
@@ -13481,7 +13477,7 @@
         <v>42705</v>
       </c>
       <c r="F78" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H78" t="s">
         <v>53</v>
@@ -13498,14 +13494,11 @@
       <c r="L78" t="s">
         <v>57</v>
       </c>
-      <c r="M78" t="s">
-        <v>202</v>
-      </c>
       <c r="N78" t="s">
         <v>19</v>
       </c>
       <c r="O78" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P78" t="s">
         <v>59</v>
@@ -13618,10 +13611,10 @@
     </row>
     <row r="79" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>232</v>
+      </c>
+      <c r="B79" t="s">
         <v>233</v>
-      </c>
-      <c r="B79" t="s">
-        <v>234</v>
       </c>
       <c r="C79" s="1">
         <v>6.5</v>
@@ -13633,7 +13626,7 @@
         <v>37083</v>
       </c>
       <c r="F79" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H79" t="s">
         <v>53</v>
@@ -13770,10 +13763,10 @@
     </row>
     <row r="80" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>232</v>
+      </c>
+      <c r="B80" t="s">
         <v>233</v>
-      </c>
-      <c r="B80" t="s">
-        <v>234</v>
       </c>
       <c r="C80" s="1">
         <v>6.125</v>
@@ -13785,7 +13778,7 @@
         <v>37351</v>
       </c>
       <c r="F80" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H80" t="s">
         <v>53</v>
@@ -13922,10 +13915,10 @@
     </row>
     <row r="81" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>232</v>
+      </c>
+      <c r="B81" t="s">
         <v>233</v>
-      </c>
-      <c r="B81" t="s">
-        <v>234</v>
       </c>
       <c r="C81" s="1">
         <v>6</v>
@@ -13937,7 +13930,7 @@
         <v>37351</v>
       </c>
       <c r="F81" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H81" t="s">
         <v>53</v>
@@ -14074,10 +14067,10 @@
     </row>
     <row r="82" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>237</v>
+      </c>
+      <c r="B82" t="s">
         <v>238</v>
-      </c>
-      <c r="B82" t="s">
-        <v>239</v>
       </c>
       <c r="C82" s="1">
         <v>10.25</v>
@@ -14089,7 +14082,7 @@
         <v>33772</v>
       </c>
       <c r="F82" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H82" t="s">
         <v>53</v>
@@ -14226,10 +14219,10 @@
     </row>
     <row r="83" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>240</v>
+      </c>
+      <c r="B83" t="s">
         <v>241</v>
-      </c>
-      <c r="B83" t="s">
-        <v>242</v>
       </c>
       <c r="C83" s="1">
         <v>10.5</v>
@@ -14241,7 +14234,7 @@
         <v>32545</v>
       </c>
       <c r="F83" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H83" t="s">
         <v>53</v>
@@ -14256,7 +14249,7 @@
         <v>70</v>
       </c>
       <c r="L83" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M83" s="3">
         <v>100281744.27671999</v>
@@ -14378,10 +14371,10 @@
     </row>
     <row r="84" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>240</v>
+      </c>
+      <c r="B84" t="s">
         <v>241</v>
-      </c>
-      <c r="B84" t="s">
-        <v>242</v>
       </c>
       <c r="C84" s="1">
         <v>6.375</v>
@@ -14393,7 +14386,7 @@
         <v>37001</v>
       </c>
       <c r="F84" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H84" t="s">
         <v>53</v>
@@ -14530,10 +14523,10 @@
     </row>
     <row r="85" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>240</v>
+      </c>
+      <c r="B85" t="s">
         <v>241</v>
-      </c>
-      <c r="B85" t="s">
-        <v>242</v>
       </c>
       <c r="C85" s="1">
         <v>6.375</v>
@@ -14545,7 +14538,7 @@
         <v>37547</v>
       </c>
       <c r="F85" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H85" t="s">
         <v>53</v>
@@ -14682,10 +14675,10 @@
     </row>
     <row r="86" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>240</v>
+      </c>
+      <c r="B86" t="s">
         <v>241</v>
-      </c>
-      <c r="B86" t="s">
-        <v>242</v>
       </c>
       <c r="C86" s="1">
         <v>8.375</v>
@@ -14697,7 +14690,7 @@
         <v>39911</v>
       </c>
       <c r="F86" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H86" t="s">
         <v>53</v>
@@ -14834,10 +14827,10 @@
     </row>
     <row r="87" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
+        <v>247</v>
+      </c>
+      <c r="B87" t="s">
         <v>248</v>
-      </c>
-      <c r="B87" t="s">
-        <v>249</v>
       </c>
       <c r="C87" s="1">
         <v>6.625</v>
@@ -14849,7 +14842,7 @@
         <v>36998</v>
       </c>
       <c r="F87" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H87" t="s">
         <v>53</v>
@@ -14986,10 +14979,10 @@
     </row>
     <row r="88" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>250</v>
+      </c>
+      <c r="B88" t="s">
         <v>251</v>
-      </c>
-      <c r="B88" t="s">
-        <v>252</v>
       </c>
       <c r="C88" s="1">
         <v>6.875</v>
@@ -15001,7 +14994,7 @@
         <v>36395</v>
       </c>
       <c r="F88" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H88" t="s">
         <v>53</v>
@@ -15138,10 +15131,10 @@
     </row>
     <row r="89" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
+        <v>250</v>
+      </c>
+      <c r="B89" t="s">
         <v>251</v>
-      </c>
-      <c r="B89" t="s">
-        <v>252</v>
       </c>
       <c r="C89" s="1">
         <v>5.625</v>
@@ -15153,7 +15146,7 @@
         <v>37915</v>
       </c>
       <c r="F89" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H89" t="s">
         <v>53</v>
@@ -15290,10 +15283,10 @@
     </row>
     <row r="90" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>254</v>
+      </c>
+      <c r="B90" t="s">
         <v>255</v>
-      </c>
-      <c r="B90" t="s">
-        <v>256</v>
       </c>
       <c r="C90" s="1">
         <v>7.8879999999999999</v>
@@ -15305,7 +15298,7 @@
         <v>36616</v>
       </c>
       <c r="F90" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H90" t="s">
         <v>53</v>
@@ -15442,10 +15435,10 @@
     </row>
     <row r="91" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>257</v>
+      </c>
+      <c r="B91" t="s">
         <v>258</v>
-      </c>
-      <c r="B91" t="s">
-        <v>259</v>
       </c>
       <c r="C91" s="1">
         <v>10</v>
@@ -15457,7 +15450,7 @@
         <v>32224</v>
       </c>
       <c r="F91" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H91" t="s">
         <v>53</v>
@@ -15594,10 +15587,10 @@
     </row>
     <row r="92" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
+        <v>260</v>
+      </c>
+      <c r="B92" t="s">
         <v>261</v>
-      </c>
-      <c r="B92" t="s">
-        <v>262</v>
       </c>
       <c r="C92" s="1">
         <v>6.375</v>
@@ -15609,7 +15602,7 @@
         <v>37202</v>
       </c>
       <c r="F92" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H92" t="s">
         <v>53</v>
@@ -15746,10 +15739,10 @@
     </row>
     <row r="93" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>260</v>
+      </c>
+      <c r="B93" t="s">
         <v>261</v>
-      </c>
-      <c r="B93" t="s">
-        <v>262</v>
       </c>
       <c r="C93" s="1">
         <v>5.625</v>
@@ -15761,7 +15754,7 @@
         <v>38070</v>
       </c>
       <c r="F93" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H93" t="s">
         <v>53</v>
@@ -15898,10 +15891,10 @@
     </row>
     <row r="94" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
+        <v>260</v>
+      </c>
+      <c r="B94" t="s">
         <v>261</v>
-      </c>
-      <c r="B94" t="s">
-        <v>262</v>
       </c>
       <c r="C94" s="1">
         <v>5.875</v>
@@ -15913,7 +15906,7 @@
         <v>39170</v>
       </c>
       <c r="F94" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H94" t="s">
         <v>53</v>
@@ -16050,10 +16043,10 @@
     </row>
     <row r="95" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
+        <v>260</v>
+      </c>
+      <c r="B95" t="s">
         <v>261</v>
-      </c>
-      <c r="B95" t="s">
-        <v>262</v>
       </c>
       <c r="C95" s="1">
         <v>6.125</v>
@@ -16065,7 +16058,7 @@
         <v>40149</v>
       </c>
       <c r="F95" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H95" t="s">
         <v>53</v>
@@ -16202,10 +16195,10 @@
     </row>
     <row r="96" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>266</v>
+      </c>
+      <c r="B96" t="s">
         <v>267</v>
-      </c>
-      <c r="B96" t="s">
-        <v>268</v>
       </c>
       <c r="C96" s="1">
         <v>6.375</v>
@@ -16217,7 +16210,7 @@
         <v>36559</v>
       </c>
       <c r="F96" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H96" t="s">
         <v>53</v>
@@ -16354,10 +16347,10 @@
     </row>
     <row r="97" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
+        <v>266</v>
+      </c>
+      <c r="B97" t="s">
         <v>267</v>
-      </c>
-      <c r="B97" t="s">
-        <v>268</v>
       </c>
       <c r="C97" s="1">
         <v>6.375</v>
@@ -16369,7 +16362,7 @@
         <v>36559</v>
       </c>
       <c r="F97" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H97" t="s">
         <v>53</v>
@@ -16506,10 +16499,10 @@
     </row>
     <row r="98" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
+        <v>270</v>
+      </c>
+      <c r="B98" t="s">
         <v>271</v>
-      </c>
-      <c r="B98" t="s">
-        <v>272</v>
       </c>
       <c r="C98" s="1">
         <v>12</v>
@@ -16521,7 +16514,7 @@
         <v>30195</v>
       </c>
       <c r="F98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H98" t="s">
         <v>53</v>
@@ -16658,10 +16651,10 @@
     </row>
     <row r="99" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
+        <v>273</v>
+      </c>
+      <c r="B99" t="s">
         <v>274</v>
-      </c>
-      <c r="B99" t="s">
-        <v>275</v>
       </c>
       <c r="C99" s="1">
         <v>10.625</v>
@@ -16673,7 +16666,7 @@
         <v>33663</v>
       </c>
       <c r="F99" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H99" t="s">
         <v>53</v>
@@ -16689,9 +16682,6 @@
       </c>
       <c r="L99" t="s">
         <v>57</v>
-      </c>
-      <c r="M99" t="s">
-        <v>202</v>
       </c>
       <c r="N99" t="s">
         <v>19</v>
@@ -16810,10 +16800,10 @@
     </row>
     <row r="100" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
+        <v>273</v>
+      </c>
+      <c r="B100" t="s">
         <v>274</v>
-      </c>
-      <c r="B100" t="s">
-        <v>275</v>
       </c>
       <c r="C100" s="1">
         <v>13.625</v>
@@ -16825,7 +16815,7 @@
         <v>33663</v>
       </c>
       <c r="F100" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H100" t="s">
         <v>53</v>
@@ -16841,9 +16831,6 @@
       </c>
       <c r="L100" t="s">
         <v>57</v>
-      </c>
-      <c r="M100" t="s">
-        <v>202</v>
       </c>
       <c r="N100" t="s">
         <v>19</v>
@@ -16962,10 +16949,10 @@
     </row>
     <row r="101" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>277</v>
+      </c>
+      <c r="B101" t="s">
         <v>278</v>
-      </c>
-      <c r="B101" t="s">
-        <v>279</v>
       </c>
       <c r="C101" s="1">
         <v>5.25</v>
@@ -16977,7 +16964,7 @@
         <v>38870</v>
       </c>
       <c r="F101" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H101" t="s">
         <v>53</v>
@@ -17114,10 +17101,10 @@
     </row>
     <row r="102" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>277</v>
+      </c>
+      <c r="B102" t="s">
         <v>278</v>
-      </c>
-      <c r="B102" t="s">
-        <v>279</v>
       </c>
       <c r="C102" s="1">
         <v>5.5</v>
@@ -17129,7 +17116,7 @@
         <v>38922</v>
       </c>
       <c r="F102" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H102" t="s">
         <v>53</v>
@@ -17266,10 +17253,10 @@
     </row>
     <row r="103" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>277</v>
+      </c>
+      <c r="B103" t="s">
         <v>278</v>
-      </c>
-      <c r="B103" t="s">
-        <v>279</v>
       </c>
       <c r="C103" s="1">
         <v>5.25</v>
@@ -17281,7 +17268,7 @@
         <v>38870</v>
       </c>
       <c r="F103" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H103" t="s">
         <v>53</v>
@@ -17418,10 +17405,10 @@
     </row>
     <row r="104" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
+        <v>277</v>
+      </c>
+      <c r="B104" t="s">
         <v>278</v>
-      </c>
-      <c r="B104" t="s">
-        <v>279</v>
       </c>
       <c r="C104" s="1">
         <v>5.5</v>
@@ -17433,7 +17420,7 @@
         <v>39825</v>
       </c>
       <c r="F104" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H104" t="s">
         <v>53</v>
@@ -17570,10 +17557,10 @@
     </row>
     <row r="105" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
+        <v>277</v>
+      </c>
+      <c r="B105" t="s">
         <v>278</v>
-      </c>
-      <c r="B105" t="s">
-        <v>279</v>
       </c>
       <c r="C105" s="1">
         <v>6.125</v>
@@ -17585,7 +17572,7 @@
         <v>39848</v>
       </c>
       <c r="F105" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H105" t="s">
         <v>53</v>
@@ -17722,10 +17709,10 @@
     </row>
     <row r="106" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
+        <v>277</v>
+      </c>
+      <c r="B106" t="s">
         <v>278</v>
-      </c>
-      <c r="B106" t="s">
-        <v>279</v>
       </c>
       <c r="C106" s="1">
         <v>6.125</v>
@@ -17737,7 +17724,7 @@
         <v>39954</v>
       </c>
       <c r="F106" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H106" t="s">
         <v>53</v>
@@ -17874,10 +17861,10 @@
     </row>
     <row r="107" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
+        <v>277</v>
+      </c>
+      <c r="B107" t="s">
         <v>278</v>
-      </c>
-      <c r="B107" t="s">
-        <v>279</v>
       </c>
       <c r="C107" s="1">
         <v>1.25</v>
@@ -17889,7 +17876,7 @@
         <v>40822</v>
       </c>
       <c r="F107" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H107" t="s">
         <v>53</v>
@@ -18026,10 +18013,10 @@
     </row>
     <row r="108" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
+        <v>286</v>
+      </c>
+      <c r="B108" t="s">
         <v>287</v>
-      </c>
-      <c r="B108" t="s">
-        <v>288</v>
       </c>
       <c r="C108" s="1">
         <v>8</v>
@@ -18041,7 +18028,7 @@
         <v>39632</v>
       </c>
       <c r="F108" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H108" t="s">
         <v>53</v>
@@ -18178,10 +18165,10 @@
     </row>
     <row r="109" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
+        <v>289</v>
+      </c>
+      <c r="B109" t="s">
         <v>290</v>
-      </c>
-      <c r="B109" t="s">
-        <v>291</v>
       </c>
       <c r="C109" s="1">
         <v>5.25</v>
@@ -18193,7 +18180,7 @@
         <v>37778</v>
       </c>
       <c r="F109" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H109" t="s">
         <v>53</v>
@@ -18330,10 +18317,10 @@
     </row>
     <row r="110" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>289</v>
+      </c>
+      <c r="B110" t="s">
         <v>290</v>
-      </c>
-      <c r="B110" t="s">
-        <v>291</v>
       </c>
       <c r="C110" s="1">
         <v>5.875</v>
@@ -18345,7 +18332,7 @@
         <v>39002</v>
       </c>
       <c r="F110" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H110" t="s">
         <v>53</v>
@@ -18482,10 +18469,10 @@
     </row>
     <row r="111" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
+        <v>293</v>
+      </c>
+      <c r="B111" t="s">
         <v>294</v>
-      </c>
-      <c r="B111" t="s">
-        <v>295</v>
       </c>
       <c r="C111" s="1">
         <v>5.625</v>
@@ -18497,7 +18484,7 @@
         <v>37761</v>
       </c>
       <c r="F111" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H111" t="s">
         <v>53</v>
@@ -18518,7 +18505,7 @@
         <v>229804921.14371997</v>
       </c>
       <c r="N111" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O111" t="s">
         <v>58</v>
@@ -18634,10 +18621,10 @@
     </row>
     <row r="112" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
+        <v>296</v>
+      </c>
+      <c r="B112" t="s">
         <v>297</v>
-      </c>
-      <c r="B112" t="s">
-        <v>298</v>
       </c>
       <c r="C112" s="1">
         <v>6.875</v>
@@ -18649,7 +18636,7 @@
         <v>37147</v>
       </c>
       <c r="F112" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H112" t="s">
         <v>53</v>
@@ -18786,10 +18773,10 @@
     </row>
     <row r="113" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
+        <v>299</v>
+      </c>
+      <c r="B113" t="s">
         <v>300</v>
-      </c>
-      <c r="B113" t="s">
-        <v>301</v>
       </c>
       <c r="C113" s="1">
         <v>3.75</v>
@@ -18801,7 +18788,7 @@
         <v>33704</v>
       </c>
       <c r="F113" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H113" t="s">
         <v>53</v>
@@ -18817,9 +18804,6 @@
       </c>
       <c r="L113" t="s">
         <v>57</v>
-      </c>
-      <c r="M113" t="s">
-        <v>202</v>
       </c>
       <c r="N113" t="s">
         <v>19</v>
@@ -18938,10 +18922,10 @@
     </row>
     <row r="114" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
+        <v>299</v>
+      </c>
+      <c r="B114" t="s">
         <v>300</v>
-      </c>
-      <c r="B114" t="s">
-        <v>301</v>
       </c>
       <c r="C114" s="1">
         <v>4.25</v>
@@ -18953,7 +18937,7 @@
         <v>33704</v>
       </c>
       <c r="F114" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H114" t="s">
         <v>53</v>
@@ -19090,10 +19074,10 @@
     </row>
     <row r="115" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
+        <v>299</v>
+      </c>
+      <c r="B115" t="s">
         <v>300</v>
-      </c>
-      <c r="B115" t="s">
-        <v>301</v>
       </c>
       <c r="C115" s="1">
         <v>5.25</v>
@@ -19105,7 +19089,7 @@
         <v>33704</v>
       </c>
       <c r="F115" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H115" t="s">
         <v>53</v>
@@ -19242,10 +19226,10 @@
     </row>
     <row r="116" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>304</v>
+      </c>
+      <c r="B116" t="s">
         <v>305</v>
-      </c>
-      <c r="B116" t="s">
-        <v>306</v>
       </c>
       <c r="C116" s="1">
         <v>3.75</v>
@@ -19257,7 +19241,7 @@
         <v>43840</v>
       </c>
       <c r="F116" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H116" t="s">
         <v>53</v>
@@ -19394,10 +19378,10 @@
     </row>
     <row r="117" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
+        <v>307</v>
+      </c>
+      <c r="B117" t="s">
         <v>308</v>
-      </c>
-      <c r="B117" t="s">
-        <v>309</v>
       </c>
       <c r="C117" s="1">
         <v>9.75</v>
@@ -19409,7 +19393,7 @@
         <v>38531</v>
       </c>
       <c r="F117" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H117" t="s">
         <v>53</v>
@@ -19546,10 +19530,10 @@
     </row>
     <row r="118" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
+        <v>310</v>
+      </c>
+      <c r="B118" t="s">
         <v>311</v>
-      </c>
-      <c r="B118" t="s">
-        <v>312</v>
       </c>
       <c r="C118" s="1">
         <v>10.25</v>
@@ -19561,7 +19545,7 @@
         <v>31929</v>
       </c>
       <c r="F118" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H118" t="s">
         <v>53</v>
@@ -19698,10 +19682,10 @@
     </row>
     <row r="119" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>313</v>
+      </c>
+      <c r="B119" t="s">
         <v>314</v>
-      </c>
-      <c r="B119" t="s">
-        <v>315</v>
       </c>
       <c r="C119" s="1">
         <v>10.25</v>
@@ -19713,7 +19697,7 @@
         <v>34800</v>
       </c>
       <c r="F119" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H119" t="s">
         <v>53</v>
@@ -19850,10 +19834,10 @@
     </row>
     <row r="120" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
+        <v>316</v>
+      </c>
+      <c r="B120" t="s">
         <v>317</v>
-      </c>
-      <c r="B120" t="s">
-        <v>318</v>
       </c>
       <c r="C120" s="1">
         <v>10.5</v>
@@ -19865,7 +19849,7 @@
         <v>32307</v>
       </c>
       <c r="F120" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H120" t="s">
         <v>53</v>
@@ -19880,7 +19864,7 @@
         <v>70</v>
       </c>
       <c r="L120" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M120" s="3">
         <v>99651534.056879997</v>
@@ -20002,10 +19986,10 @@
     </row>
     <row r="121" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
+        <v>316</v>
+      </c>
+      <c r="B121" t="s">
         <v>317</v>
-      </c>
-      <c r="B121" t="s">
-        <v>318</v>
       </c>
       <c r="C121" s="1">
         <v>7</v>
@@ -20017,7 +20001,7 @@
         <v>36460</v>
       </c>
       <c r="F121" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H121" t="s">
         <v>53</v>
@@ -20154,10 +20138,10 @@
     </row>
     <row r="122" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>320</v>
+      </c>
+      <c r="B122" t="s">
         <v>321</v>
-      </c>
-      <c r="B122" t="s">
-        <v>322</v>
       </c>
       <c r="C122" s="1">
         <v>5</v>
@@ -20169,7 +20153,7 @@
         <v>41725</v>
       </c>
       <c r="F122" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H122" t="s">
         <v>53</v>
@@ -20185,9 +20169,6 @@
       </c>
       <c r="L122" t="s">
         <v>65</v>
-      </c>
-      <c r="M122" t="s">
-        <v>202</v>
       </c>
       <c r="N122" t="s">
         <v>19</v>
@@ -20306,10 +20287,10 @@
     </row>
     <row r="123" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>323</v>
+      </c>
+      <c r="B123" t="s">
         <v>324</v>
-      </c>
-      <c r="B123" t="s">
-        <v>325</v>
       </c>
       <c r="C123" s="1">
         <v>6.125</v>
@@ -20321,7 +20302,7 @@
         <v>37214</v>
       </c>
       <c r="F123" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H123" t="s">
         <v>53</v>
@@ -20458,10 +20439,10 @@
     </row>
     <row r="124" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
+        <v>323</v>
+      </c>
+      <c r="B124" t="s">
         <v>324</v>
-      </c>
-      <c r="B124" t="s">
-        <v>325</v>
       </c>
       <c r="C124" s="1">
         <v>5.75</v>
@@ -20473,7 +20454,7 @@
         <v>38807</v>
       </c>
       <c r="F124" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H124" t="s">
         <v>53</v>
@@ -20610,10 +20591,10 @@
     </row>
     <row r="125" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
+        <v>327</v>
+      </c>
+      <c r="B125" t="s">
         <v>328</v>
-      </c>
-      <c r="B125" t="s">
-        <v>329</v>
       </c>
       <c r="C125" s="1">
         <v>12.375</v>
@@ -20625,7 +20606,7 @@
         <v>33569</v>
       </c>
       <c r="F125" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H125" t="s">
         <v>53</v>
@@ -20762,10 +20743,10 @@
     </row>
     <row r="126" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>330</v>
+      </c>
+      <c r="B126" t="s">
         <v>331</v>
-      </c>
-      <c r="B126" t="s">
-        <v>332</v>
       </c>
       <c r="C126" s="1">
         <v>5.5</v>
@@ -20777,7 +20758,7 @@
         <v>39876</v>
       </c>
       <c r="F126" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H126" t="s">
         <v>53</v>
@@ -20914,10 +20895,10 @@
     </row>
     <row r="127" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
+        <v>333</v>
+      </c>
+      <c r="B127" t="s">
         <v>334</v>
-      </c>
-      <c r="B127" t="s">
-        <v>335</v>
       </c>
       <c r="C127" s="1">
         <v>6.125</v>
@@ -20929,7 +20910,7 @@
         <v>36146</v>
       </c>
       <c r="F127" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H127" t="s">
         <v>53</v>
@@ -21066,10 +21047,10 @@
     </row>
     <row r="128" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
+        <v>333</v>
+      </c>
+      <c r="B128" t="s">
         <v>334</v>
-      </c>
-      <c r="B128" t="s">
-        <v>335</v>
       </c>
       <c r="C128" s="1">
         <v>6.5</v>
@@ -21081,7 +21062,7 @@
         <v>36377</v>
       </c>
       <c r="F128" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H128" t="s">
         <v>53</v>
@@ -21218,10 +21199,10 @@
     </row>
     <row r="129" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
+        <v>337</v>
+      </c>
+      <c r="B129" t="s">
         <v>338</v>
-      </c>
-      <c r="B129" t="s">
-        <v>339</v>
       </c>
       <c r="C129" s="1">
         <v>5.5</v>
@@ -21233,7 +21214,7 @@
         <v>39100</v>
       </c>
       <c r="F129" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H129" t="s">
         <v>53</v>
@@ -21370,10 +21351,10 @@
     </row>
     <row r="130" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>340</v>
+      </c>
+      <c r="B130" t="s">
         <v>341</v>
-      </c>
-      <c r="B130" t="s">
-        <v>342</v>
       </c>
       <c r="C130" s="1">
         <v>2</v>
@@ -21385,7 +21366,7 @@
         <v>41060</v>
       </c>
       <c r="F130" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H130" t="s">
         <v>53</v>
@@ -21409,7 +21390,7 @@
         <v>19</v>
       </c>
       <c r="O130" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P130" t="s">
         <v>59</v>
@@ -21522,10 +21503,10 @@
     </row>
     <row r="131" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
+        <v>343</v>
+      </c>
+      <c r="B131" t="s">
         <v>344</v>
-      </c>
-      <c r="B131" t="s">
-        <v>345</v>
       </c>
       <c r="C131" s="1">
         <v>10.375</v>
@@ -21537,7 +21518,7 @@
         <v>32623</v>
       </c>
       <c r="F131" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H131" t="s">
         <v>53</v>
@@ -21674,10 +21655,10 @@
     </row>
     <row r="132" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
+        <v>346</v>
+      </c>
+      <c r="B132" t="s">
         <v>347</v>
-      </c>
-      <c r="B132" t="s">
-        <v>348</v>
       </c>
       <c r="C132" s="1">
         <v>5.75</v>
@@ -21689,7 +21670,7 @@
         <v>38645</v>
       </c>
       <c r="F132" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H132" t="s">
         <v>53</v>
@@ -21826,10 +21807,10 @@
     </row>
     <row r="133" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
+        <v>346</v>
+      </c>
+      <c r="B133" t="s">
         <v>347</v>
-      </c>
-      <c r="B133" t="s">
-        <v>348</v>
       </c>
       <c r="C133" s="1">
         <v>5.75</v>
@@ -21841,7 +21822,7 @@
         <v>38645</v>
       </c>
       <c r="F133" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H133" t="s">
         <v>53</v>
@@ -21978,10 +21959,10 @@
     </row>
     <row r="134" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
+        <v>350</v>
+      </c>
+      <c r="B134" t="s">
         <v>351</v>
-      </c>
-      <c r="B134" t="s">
-        <v>352</v>
       </c>
       <c r="C134" s="1">
         <v>7.75</v>
@@ -21993,7 +21974,7 @@
         <v>36350</v>
       </c>
       <c r="F134" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H134" t="s">
         <v>53</v>
@@ -22017,7 +21998,7 @@
         <v>74</v>
       </c>
       <c r="O134" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P134" t="s">
         <v>59</v>
@@ -22130,10 +22111,10 @@
     </row>
     <row r="135" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
+        <v>350</v>
+      </c>
+      <c r="B135" t="s">
         <v>351</v>
-      </c>
-      <c r="B135" t="s">
-        <v>352</v>
       </c>
       <c r="C135" s="1">
         <v>7.75</v>
@@ -22145,7 +22126,7 @@
         <v>36517</v>
       </c>
       <c r="F135" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H135" t="s">
         <v>53</v>
@@ -22169,7 +22150,7 @@
         <v>74</v>
       </c>
       <c r="O135" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P135" t="s">
         <v>59</v>
@@ -22282,10 +22263,10 @@
     </row>
     <row r="136" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
+        <v>350</v>
+      </c>
+      <c r="B136" t="s">
         <v>351</v>
-      </c>
-      <c r="B136" t="s">
-        <v>352</v>
       </c>
       <c r="C136" s="1">
         <v>7.75</v>
@@ -22297,7 +22278,7 @@
         <v>36350</v>
       </c>
       <c r="F136" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H136" t="s">
         <v>53</v>
@@ -22321,7 +22302,7 @@
         <v>19</v>
       </c>
       <c r="O136" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P136" t="s">
         <v>59</v>
@@ -22434,10 +22415,10 @@
     </row>
     <row r="137" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
+        <v>350</v>
+      </c>
+      <c r="B137" t="s">
         <v>351</v>
-      </c>
-      <c r="B137" t="s">
-        <v>352</v>
       </c>
       <c r="C137" s="1">
         <v>7.75</v>
@@ -22449,7 +22430,7 @@
         <v>36350</v>
       </c>
       <c r="F137" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H137" t="s">
         <v>53</v>
@@ -22473,7 +22454,7 @@
         <v>19</v>
       </c>
       <c r="O137" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P137" t="s">
         <v>59</v>
@@ -22586,10 +22567,10 @@
     </row>
     <row r="138" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
+        <v>350</v>
+      </c>
+      <c r="B138" t="s">
         <v>351</v>
-      </c>
-      <c r="B138" t="s">
-        <v>352</v>
       </c>
       <c r="C138" s="1">
         <v>7.75</v>
@@ -22601,7 +22582,7 @@
         <v>36350</v>
       </c>
       <c r="F138" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H138" t="s">
         <v>53</v>
@@ -22625,7 +22606,7 @@
         <v>19</v>
       </c>
       <c r="O138" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P138" t="s">
         <v>59</v>
@@ -22738,10 +22719,10 @@
     </row>
     <row r="139" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
+        <v>350</v>
+      </c>
+      <c r="B139" t="s">
         <v>351</v>
-      </c>
-      <c r="B139" t="s">
-        <v>352</v>
       </c>
       <c r="C139" s="1">
         <v>2.875</v>
@@ -22753,7 +22734,7 @@
         <v>41967</v>
       </c>
       <c r="F139" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H139" t="s">
         <v>53</v>
@@ -22777,7 +22758,7 @@
         <v>19</v>
       </c>
       <c r="O139" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P139" t="s">
         <v>59</v>
@@ -22890,10 +22871,10 @@
     </row>
     <row r="140" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
+        <v>358</v>
+      </c>
+      <c r="B140" t="s">
         <v>359</v>
-      </c>
-      <c r="B140" t="s">
-        <v>360</v>
       </c>
       <c r="C140" s="1">
         <v>9.875</v>
@@ -22905,7 +22886,7 @@
         <v>31470</v>
       </c>
       <c r="F140" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H140" t="s">
         <v>53</v>
@@ -22920,7 +22901,7 @@
         <v>70</v>
       </c>
       <c r="L140" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M140" s="3">
         <v>71035049.651040003</v>
@@ -23042,10 +23023,10 @@
     </row>
     <row r="141" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
+        <v>361</v>
+      </c>
+      <c r="B141" t="s">
         <v>362</v>
-      </c>
-      <c r="B141" t="s">
-        <v>363</v>
       </c>
       <c r="C141" s="1">
         <v>5.125</v>
@@ -23057,7 +23038,7 @@
         <v>36178</v>
       </c>
       <c r="F141" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H141" t="s">
         <v>53</v>
@@ -23194,10 +23175,10 @@
     </row>
     <row r="142" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
+        <v>361</v>
+      </c>
+      <c r="B142" t="s">
         <v>362</v>
-      </c>
-      <c r="B142" t="s">
-        <v>363</v>
       </c>
       <c r="C142" s="1">
         <v>5.125</v>
@@ -23209,7 +23190,7 @@
         <v>36220</v>
       </c>
       <c r="F142" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H142" t="s">
         <v>53</v>
@@ -23346,10 +23327,10 @@
     </row>
     <row r="143" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
+        <v>361</v>
+      </c>
+      <c r="B143" t="s">
         <v>362</v>
-      </c>
-      <c r="B143" t="s">
-        <v>363</v>
       </c>
       <c r="C143" s="1">
         <v>5.125</v>
@@ -23361,7 +23342,7 @@
         <v>36236</v>
       </c>
       <c r="F143" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H143" t="s">
         <v>53</v>
@@ -23498,10 +23479,10 @@
     </row>
     <row r="144" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
+        <v>361</v>
+      </c>
+      <c r="B144" t="s">
         <v>362</v>
-      </c>
-      <c r="B144" t="s">
-        <v>363</v>
       </c>
       <c r="C144" s="1">
         <v>4</v>
@@ -23513,7 +23494,7 @@
         <v>36777</v>
       </c>
       <c r="F144" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H144" t="s">
         <v>53</v>
@@ -23650,10 +23631,10 @@
     </row>
     <row r="145" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>361</v>
+      </c>
+      <c r="B145" t="s">
         <v>362</v>
-      </c>
-      <c r="B145" t="s">
-        <v>363</v>
       </c>
       <c r="C145" s="1">
         <v>6.625</v>
@@ -23665,7 +23646,7 @@
         <v>36811</v>
       </c>
       <c r="F145" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H145" t="s">
         <v>53</v>
@@ -23802,10 +23783,10 @@
     </row>
     <row r="146" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
+        <v>361</v>
+      </c>
+      <c r="B146" t="s">
         <v>362</v>
-      </c>
-      <c r="B146" t="s">
-        <v>363</v>
       </c>
       <c r="C146" s="1">
         <v>6</v>
@@ -23817,7 +23798,7 @@
         <v>37055</v>
       </c>
       <c r="F146" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H146" t="s">
         <v>53</v>
@@ -23954,10 +23935,10 @@
     </row>
     <row r="147" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
+        <v>361</v>
+      </c>
+      <c r="B147" t="s">
         <v>362</v>
-      </c>
-      <c r="B147" t="s">
-        <v>363</v>
       </c>
       <c r="C147" s="1">
         <v>3.3220000000000001</v>
@@ -23969,7 +23950,7 @@
         <v>37603</v>
       </c>
       <c r="F147" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H147" t="s">
         <v>53</v>
@@ -24106,10 +24087,10 @@
     </row>
     <row r="148" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
+        <v>361</v>
+      </c>
+      <c r="B148" t="s">
         <v>362</v>
-      </c>
-      <c r="B148" t="s">
-        <v>363</v>
       </c>
       <c r="C148" s="1">
         <v>5.5</v>
@@ -24121,7 +24102,7 @@
         <v>37603</v>
       </c>
       <c r="F148" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H148" t="s">
         <v>53</v>
@@ -24258,10 +24239,10 @@
     </row>
     <row r="149" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
+        <v>361</v>
+      </c>
+      <c r="B149" t="s">
         <v>362</v>
-      </c>
-      <c r="B149" t="s">
-        <v>363</v>
       </c>
       <c r="C149" s="1">
         <v>6</v>
@@ -24273,7 +24254,7 @@
         <v>37055</v>
       </c>
       <c r="F149" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H149" t="s">
         <v>53</v>
@@ -24410,10 +24391,10 @@
     </row>
     <row r="150" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
+        <v>361</v>
+      </c>
+      <c r="B150" t="s">
         <v>362</v>
-      </c>
-      <c r="B150" t="s">
-        <v>363</v>
       </c>
       <c r="C150" s="1">
         <v>5</v>
@@ -24425,7 +24406,7 @@
         <v>39373</v>
       </c>
       <c r="F150" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H150" t="s">
         <v>53</v>
@@ -24562,10 +24543,10 @@
     </row>
     <row r="151" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
+        <v>361</v>
+      </c>
+      <c r="B151" t="s">
         <v>362</v>
-      </c>
-      <c r="B151" t="s">
-        <v>363</v>
       </c>
       <c r="C151" s="1">
         <v>5</v>
@@ -24577,7 +24558,7 @@
         <v>39735</v>
       </c>
       <c r="F151" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H151" t="s">
         <v>53</v>
@@ -24714,10 +24695,10 @@
     </row>
     <row r="152" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
+        <v>361</v>
+      </c>
+      <c r="B152" t="s">
         <v>362</v>
-      </c>
-      <c r="B152" t="s">
-        <v>363</v>
       </c>
       <c r="C152" s="1">
         <v>5</v>
@@ -24729,7 +24710,7 @@
         <v>39868</v>
       </c>
       <c r="F152" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H152" t="s">
         <v>53</v>
@@ -24866,10 +24847,10 @@
     </row>
     <row r="153" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
+        <v>361</v>
+      </c>
+      <c r="B153" t="s">
         <v>362</v>
-      </c>
-      <c r="B153" t="s">
-        <v>363</v>
       </c>
       <c r="C153" s="1">
         <v>6.125</v>
@@ -24881,7 +24862,7 @@
         <v>39868</v>
       </c>
       <c r="F153" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H153" t="s">
         <v>53</v>
@@ -24923,105 +24904,105 @@
         <v>1</v>
       </c>
       <c r="U153" t="s">
+        <v>376</v>
+      </c>
+      <c r="V153" t="s">
+        <v>19</v>
+      </c>
+      <c r="W153" t="s">
         <v>377</v>
       </c>
-      <c r="V153" t="s">
-        <v>19</v>
-      </c>
-      <c r="W153" t="s">
+      <c r="X153" t="s">
+        <v>377</v>
+      </c>
+      <c r="Y153" t="s">
         <v>378</v>
       </c>
-      <c r="X153" t="s">
-        <v>378</v>
-      </c>
-      <c r="Y153" t="s">
+      <c r="Z153" t="s">
         <v>379</v>
       </c>
-      <c r="Z153" t="s">
+      <c r="AA153" t="s">
         <v>380</v>
       </c>
-      <c r="AA153" t="s">
+      <c r="AB153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF153" t="s">
         <v>381</v>
       </c>
-      <c r="AB153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF153" t="s">
+      <c r="AG153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS153" t="s">
+        <v>377</v>
+      </c>
+      <c r="AT153" t="s">
         <v>382</v>
       </c>
-      <c r="AG153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AM153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AN153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AO153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AP153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AQ153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AR153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AS153" t="s">
-        <v>378</v>
-      </c>
-      <c r="AT153" t="s">
+      <c r="AU153" t="s">
         <v>383</v>
       </c>
-      <c r="AU153" t="s">
+      <c r="AV153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW153" t="s">
         <v>384</v>
       </c>
-      <c r="AV153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AW153" t="s">
+      <c r="AX153" t="s">
         <v>385</v>
       </c>
-      <c r="AX153" t="s">
+      <c r="AY153" t="s">
         <v>386</v>
-      </c>
-      <c r="AY153" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="154" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
+        <v>387</v>
+      </c>
+      <c r="B154" t="s">
         <v>388</v>
-      </c>
-      <c r="B154" t="s">
-        <v>389</v>
       </c>
       <c r="C154" s="1">
         <v>3.5</v>
@@ -25033,7 +25014,7 @@
         <v>42124</v>
       </c>
       <c r="F154" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H154" t="s">
         <v>53</v>
@@ -25170,10 +25151,10 @@
     </row>
     <row r="155" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
+        <v>390</v>
+      </c>
+      <c r="B155" t="s">
         <v>391</v>
-      </c>
-      <c r="B155" t="s">
-        <v>392</v>
       </c>
       <c r="C155" s="1">
         <v>7.75</v>
@@ -25185,7 +25166,7 @@
         <v>40290</v>
       </c>
       <c r="F155" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H155" t="s">
         <v>53</v>
@@ -25322,10 +25303,10 @@
     </row>
     <row r="156" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
+        <v>393</v>
+      </c>
+      <c r="B156" t="s">
         <v>394</v>
-      </c>
-      <c r="B156" t="s">
-        <v>395</v>
       </c>
       <c r="C156" s="1">
         <v>4.375</v>
@@ -25337,7 +25318,7 @@
         <v>41897</v>
       </c>
       <c r="F156" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H156" t="s">
         <v>53</v>
@@ -25474,10 +25455,10 @@
     </row>
     <row r="157" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
+        <v>396</v>
+      </c>
+      <c r="B157" t="s">
         <v>397</v>
-      </c>
-      <c r="B157" t="s">
-        <v>398</v>
       </c>
       <c r="C157" s="1">
         <v>11</v>
@@ -25489,7 +25470,7 @@
         <v>31462</v>
       </c>
       <c r="F157" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H157" t="s">
         <v>53</v>
@@ -25626,10 +25607,10 @@
     </row>
     <row r="158" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
+        <v>399</v>
+      </c>
+      <c r="B158" t="s">
         <v>400</v>
-      </c>
-      <c r="B158" t="s">
-        <v>401</v>
       </c>
       <c r="C158" s="1">
         <v>6.5</v>
@@ -25641,7 +25622,7 @@
         <v>40140</v>
       </c>
       <c r="F158" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H158" t="s">
         <v>53</v>
@@ -25778,10 +25759,10 @@
     </row>
     <row r="159" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
+        <v>402</v>
+      </c>
+      <c r="B159" t="s">
         <v>403</v>
-      </c>
-      <c r="B159" t="s">
-        <v>404</v>
       </c>
       <c r="C159" s="1">
         <v>5.25</v>
@@ -25793,7 +25774,7 @@
         <v>37551</v>
       </c>
       <c r="F159" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H159" t="s">
         <v>53</v>
@@ -25930,10 +25911,10 @@
     </row>
     <row r="160" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
+        <v>402</v>
+      </c>
+      <c r="B160" t="s">
         <v>403</v>
-      </c>
-      <c r="B160" t="s">
-        <v>404</v>
       </c>
       <c r="C160" s="1">
         <v>5.625</v>
@@ -25945,7 +25926,7 @@
         <v>37610</v>
       </c>
       <c r="F160" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H160" t="s">
         <v>53</v>
@@ -26082,10 +26063,10 @@
     </row>
     <row r="161" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
+        <v>402</v>
+      </c>
+      <c r="B161" t="s">
         <v>403</v>
-      </c>
-      <c r="B161" t="s">
-        <v>404</v>
       </c>
       <c r="C161" s="1">
         <v>5.375</v>
@@ -26097,7 +26078,7 @@
         <v>37755</v>
       </c>
       <c r="F161" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H161" t="s">
         <v>53</v>
@@ -26234,10 +26215,10 @@
     </row>
     <row r="162" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
+        <v>402</v>
+      </c>
+      <c r="B162" t="s">
         <v>403</v>
-      </c>
-      <c r="B162" t="s">
-        <v>404</v>
       </c>
       <c r="C162" s="1">
         <v>5.625</v>
@@ -26249,7 +26230,7 @@
         <v>37610</v>
       </c>
       <c r="F162" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H162" t="s">
         <v>53</v>
@@ -26386,10 +26367,10 @@
     </row>
     <row r="163" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
+        <v>402</v>
+      </c>
+      <c r="B163" t="s">
         <v>403</v>
-      </c>
-      <c r="B163" t="s">
-        <v>404</v>
       </c>
       <c r="C163" s="1">
         <v>1.5865</v>
@@ -26401,7 +26382,7 @@
         <v>38945</v>
       </c>
       <c r="F163" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H163" t="s">
         <v>53</v>
@@ -26538,10 +26519,10 @@
     </row>
     <row r="164" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
+        <v>402</v>
+      </c>
+      <c r="B164" t="s">
         <v>403</v>
-      </c>
-      <c r="B164" t="s">
-        <v>404</v>
       </c>
       <c r="C164" s="1">
         <v>6.125</v>
@@ -26553,7 +26534,7 @@
         <v>39811</v>
       </c>
       <c r="F164" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H164" t="s">
         <v>53</v>
@@ -26690,10 +26671,10 @@
     </row>
     <row r="165" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>402</v>
+      </c>
+      <c r="B165" t="s">
         <v>403</v>
-      </c>
-      <c r="B165" t="s">
-        <v>404</v>
       </c>
       <c r="C165" s="1">
         <v>6.125</v>
@@ -26705,7 +26686,7 @@
         <v>39829</v>
       </c>
       <c r="F165" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H165" t="s">
         <v>53</v>
@@ -26842,10 +26823,10 @@
     </row>
     <row r="166" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
+        <v>402</v>
+      </c>
+      <c r="B166" t="s">
         <v>403</v>
-      </c>
-      <c r="B166" t="s">
-        <v>404</v>
       </c>
       <c r="C166" s="1">
         <v>6.125</v>
@@ -26857,7 +26838,7 @@
         <v>39862</v>
       </c>
       <c r="F166" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H166" t="s">
         <v>53</v>
@@ -26994,10 +26975,10 @@
     </row>
     <row r="167" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
+        <v>402</v>
+      </c>
+      <c r="B167" t="s">
         <v>403</v>
-      </c>
-      <c r="B167" t="s">
-        <v>404</v>
       </c>
       <c r="C167" s="1">
         <v>5.75</v>
@@ -27009,7 +26990,7 @@
         <v>39897</v>
       </c>
       <c r="F167" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H167" t="s">
         <v>53</v>
@@ -27146,10 +27127,10 @@
     </row>
     <row r="168" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
+        <v>402</v>
+      </c>
+      <c r="B168" t="s">
         <v>403</v>
-      </c>
-      <c r="B168" t="s">
-        <v>404</v>
       </c>
       <c r="C168" s="1">
         <v>5.75</v>
@@ -27161,7 +27142,7 @@
         <v>39976</v>
       </c>
       <c r="F168" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H168" t="s">
         <v>53</v>
@@ -27298,10 +27279,10 @@
     </row>
     <row r="169" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
+        <v>402</v>
+      </c>
+      <c r="B169" t="s">
         <v>403</v>
-      </c>
-      <c r="B169" t="s">
-        <v>404</v>
       </c>
       <c r="C169" s="1">
         <v>6.125</v>
@@ -27313,7 +27294,7 @@
         <v>39993</v>
       </c>
       <c r="F169" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H169" t="s">
         <v>53</v>
@@ -27450,10 +27431,10 @@
     </row>
     <row r="170" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
+        <v>415</v>
+      </c>
+      <c r="B170" t="s">
         <v>416</v>
-      </c>
-      <c r="B170" t="s">
-        <v>417</v>
       </c>
       <c r="C170" s="1">
         <v>2.544</v>
@@ -27465,7 +27446,7 @@
         <v>43852</v>
       </c>
       <c r="F170" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H170" t="s">
         <v>53</v>
@@ -27602,10 +27583,10 @@
     </row>
     <row r="171" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
+        <v>418</v>
+      </c>
+      <c r="B171" t="s">
         <v>419</v>
-      </c>
-      <c r="B171" t="s">
-        <v>420</v>
       </c>
       <c r="C171" s="1">
         <v>4.75</v>
@@ -27617,7 +27598,7 @@
         <v>37650</v>
       </c>
       <c r="F171" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H171" t="s">
         <v>53</v>
@@ -27754,10 +27735,10 @@
     </row>
     <row r="172" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
+        <v>421</v>
+      </c>
+      <c r="B172" t="s">
         <v>422</v>
-      </c>
-      <c r="B172" t="s">
-        <v>423</v>
       </c>
       <c r="C172" s="1">
         <v>8.125</v>
@@ -27769,7 +27750,7 @@
         <v>38085</v>
       </c>
       <c r="F172" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H172" t="s">
         <v>53</v>
@@ -27906,10 +27887,10 @@
     </row>
     <row r="173" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
+        <v>424</v>
+      </c>
+      <c r="B173" t="s">
         <v>425</v>
-      </c>
-      <c r="B173" t="s">
-        <v>426</v>
       </c>
       <c r="C173" s="1">
         <v>7.125</v>
@@ -27921,7 +27902,7 @@
         <v>40129</v>
       </c>
       <c r="F173" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H173" t="s">
         <v>53</v>
@@ -28058,10 +28039,10 @@
     </row>
     <row r="174" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
+        <v>424</v>
+      </c>
+      <c r="B174" t="s">
         <v>425</v>
-      </c>
-      <c r="B174" t="s">
-        <v>426</v>
       </c>
       <c r="C174" s="1">
         <v>4.25</v>
@@ -28073,7 +28054,7 @@
         <v>41430</v>
       </c>
       <c r="F174" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H174" t="s">
         <v>53</v>
@@ -28210,10 +28191,10 @@
     </row>
     <row r="175" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
+        <v>424</v>
+      </c>
+      <c r="B175" t="s">
         <v>425</v>
-      </c>
-      <c r="B175" t="s">
-        <v>426</v>
       </c>
       <c r="C175" s="1">
         <v>4.875</v>
@@ -28225,7 +28206,7 @@
         <v>42517</v>
       </c>
       <c r="F175" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H175" t="s">
         <v>53</v>
@@ -28246,7 +28227,7 @@
         <v>349793325.52667999</v>
       </c>
       <c r="N175" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O175" t="s">
         <v>138</v>
@@ -28362,10 +28343,10 @@
     </row>
     <row r="176" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
+        <v>429</v>
+      </c>
+      <c r="B176" t="s">
         <v>430</v>
-      </c>
-      <c r="B176" t="s">
-        <v>431</v>
       </c>
       <c r="C176" s="1">
         <v>6</v>
@@ -28377,7 +28358,7 @@
         <v>37243</v>
       </c>
       <c r="F176" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H176" t="s">
         <v>53</v>
@@ -28514,10 +28495,10 @@
     </row>
     <row r="177" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
+        <v>429</v>
+      </c>
+      <c r="B177" t="s">
         <v>430</v>
-      </c>
-      <c r="B177" t="s">
-        <v>431</v>
       </c>
       <c r="C177" s="1">
         <v>4.625</v>
@@ -28529,7 +28510,7 @@
         <v>40885</v>
       </c>
       <c r="F177" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H177" t="s">
         <v>53</v>
@@ -28666,10 +28647,10 @@
     </row>
     <row r="178" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
+        <v>433</v>
+      </c>
+      <c r="B178" t="s">
         <v>434</v>
-      </c>
-      <c r="B178" t="s">
-        <v>435</v>
       </c>
       <c r="C178" s="1">
         <v>6</v>
@@ -28681,7 +28662,7 @@
         <v>41191</v>
       </c>
       <c r="F178" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H178" t="s">
         <v>53</v>
@@ -28818,10 +28799,10 @@
     </row>
     <row r="179" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
+        <v>436</v>
+      </c>
+      <c r="B179" t="s">
         <v>437</v>
-      </c>
-      <c r="B179" t="s">
-        <v>438</v>
       </c>
       <c r="C179" s="1">
         <v>6</v>
@@ -28833,7 +28814,7 @@
         <v>39176</v>
       </c>
       <c r="F179" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H179" t="s">
         <v>53</v>
@@ -28970,10 +28951,10 @@
     </row>
     <row r="180" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
+        <v>439</v>
+      </c>
+      <c r="B180" t="s">
         <v>440</v>
-      </c>
-      <c r="B180" t="s">
-        <v>441</v>
       </c>
       <c r="C180" s="1">
         <v>0</v>
@@ -28985,7 +28966,7 @@
         <v>42164</v>
       </c>
       <c r="F180" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H180" t="s">
         <v>53</v>
@@ -29001,9 +28982,6 @@
       </c>
       <c r="L180" t="s">
         <v>65</v>
-      </c>
-      <c r="M180" t="s">
-        <v>202</v>
       </c>
       <c r="N180" t="s">
         <v>19</v>
@@ -29122,10 +29100,10 @@
     </row>
     <row r="181" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
+        <v>439</v>
+      </c>
+      <c r="B181" t="s">
         <v>440</v>
-      </c>
-      <c r="B181" t="s">
-        <v>441</v>
       </c>
       <c r="C181" s="1">
         <v>0</v>
@@ -29137,7 +29115,7 @@
         <v>42164</v>
       </c>
       <c r="F181" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H181" t="s">
         <v>53</v>
@@ -29153,9 +29131,6 @@
       </c>
       <c r="L181" t="s">
         <v>65</v>
-      </c>
-      <c r="M181" t="s">
-        <v>202</v>
       </c>
       <c r="N181" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
fixed issues with data
</commit_message>
<xml_diff>
--- a/GBP Bonds/Master List of Bonds/Service Companies -disc.xlsx
+++ b/GBP Bonds/Master List of Bonds/Service Companies -disc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renea\OneDrive\Documents\University of Bath\13. Dissertation\Data\GBP Bonds\Master List of Bonds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renea\Documents\University of Bath\13. Dissertation\EstimatingCreditSpreadsViaMachineLearning\GBP Bonds\Master List of Bonds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66B041E-078A-4253-B1FF-6BF54279C802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B5BAE7-EB64-4DAA-8C64-1AEE1F88DAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Search Results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8330" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8330" uniqueCount="442">
   <si>
     <t>Issuer</t>
   </si>
@@ -1058,9 +1058,6 @@
   </si>
   <si>
     <t>GB0000833136</t>
-  </si>
-  <si>
-    <t>Sky Group Finance Ltd</t>
   </si>
   <si>
     <t>CMCSKG</t>
@@ -1734,32 +1731,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
-    <col min="2" max="2" width="16.69921875" customWidth="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="19.19921875" customWidth="1"/>
+    <col min="4" max="4" width="19.25" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="23.296875" customWidth="1"/>
+    <col min="7" max="7" width="23.25" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="21.69921875" customWidth="1"/>
+    <col min="9" max="9" width="21.75" customWidth="1"/>
     <col min="10" max="10" width="25" customWidth="1"/>
     <col min="11" max="11" width="35" customWidth="1"/>
-    <col min="12" max="12" width="33.296875" customWidth="1"/>
+    <col min="12" max="12" width="33.25" customWidth="1"/>
     <col min="13" max="13" width="25" customWidth="1"/>
-    <col min="14" max="14" width="20.796875" customWidth="1"/>
+    <col min="14" max="14" width="20.75" customWidth="1"/>
     <col min="15" max="15" width="25" customWidth="1"/>
     <col min="16" max="16" width="12.5" customWidth="1"/>
-    <col min="17" max="19" width="11.69921875" customWidth="1"/>
-    <col min="20" max="51" width="16.69921875" customWidth="1"/>
+    <col min="17" max="19" width="11.75" customWidth="1"/>
+    <col min="20" max="51" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1914,7 +1911,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -2066,7 +2063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -2218,7 +2215,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -2370,7 +2367,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -2522,7 +2519,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -2674,7 +2671,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -2826,7 +2823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -2978,7 +2975,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -3130,7 +3127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -3282,7 +3279,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -3434,7 +3431,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -3586,7 +3583,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>89</v>
       </c>
@@ -3738,7 +3735,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -3890,7 +3887,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -4042,7 +4039,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -4194,7 +4191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -4346,7 +4343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>102</v>
       </c>
@@ -4498,7 +4495,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -4650,7 +4647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>108</v>
       </c>
@@ -4802,7 +4799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -4954,7 +4951,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>112</v>
       </c>
@@ -5106,7 +5103,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>115</v>
       </c>
@@ -5258,7 +5255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -5410,7 +5407,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>122</v>
       </c>
@@ -5562,7 +5559,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>125</v>
       </c>
@@ -5714,7 +5711,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -5866,7 +5863,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>132</v>
       </c>
@@ -6018,7 +6015,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>135</v>
       </c>
@@ -6170,7 +6167,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -6322,7 +6319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>139</v>
       </c>
@@ -6474,7 +6471,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>143</v>
       </c>
@@ -6626,7 +6623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -6778,7 +6775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>143</v>
       </c>
@@ -6930,7 +6927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>143</v>
       </c>
@@ -7082,7 +7079,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -7234,7 +7231,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -7386,7 +7383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -7538,7 +7535,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>154</v>
       </c>
@@ -7690,7 +7687,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>154</v>
       </c>
@@ -7842,7 +7839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -7994,7 +7991,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>159</v>
       </c>
@@ -8146,7 +8143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>159</v>
       </c>
@@ -8298,7 +8295,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>159</v>
       </c>
@@ -8450,7 +8447,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>159</v>
       </c>
@@ -8602,7 +8599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>159</v>
       </c>
@@ -8754,7 +8751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>159</v>
       </c>
@@ -8906,7 +8903,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>167</v>
       </c>
@@ -9058,7 +9055,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>170</v>
       </c>
@@ -9210,7 +9207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>170</v>
       </c>
@@ -9362,7 +9359,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>170</v>
       </c>
@@ -9514,7 +9511,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>170</v>
       </c>
@@ -9666,7 +9663,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -9818,7 +9815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>170</v>
       </c>
@@ -9970,7 +9967,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>170</v>
       </c>
@@ -10122,7 +10119,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>180</v>
       </c>
@@ -10274,7 +10271,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>183</v>
       </c>
@@ -10426,7 +10423,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>183</v>
       </c>
@@ -10578,7 +10575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>183</v>
       </c>
@@ -10730,7 +10727,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>188</v>
       </c>
@@ -10882,7 +10879,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>191</v>
       </c>
@@ -11034,7 +11031,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>191</v>
       </c>
@@ -11186,7 +11183,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>191</v>
       </c>
@@ -11338,7 +11335,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>196</v>
       </c>
@@ -11490,7 +11487,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>199</v>
       </c>
@@ -11639,7 +11636,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>199</v>
       </c>
@@ -11791,7 +11788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>199</v>
       </c>
@@ -11943,7 +11940,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>204</v>
       </c>
@@ -12095,7 +12092,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>207</v>
       </c>
@@ -12247,7 +12244,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>212</v>
       </c>
@@ -12399,7 +12396,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>215</v>
       </c>
@@ -12551,7 +12548,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>218</v>
       </c>
@@ -12703,7 +12700,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>221</v>
       </c>
@@ -12855,7 +12852,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>221</v>
       </c>
@@ -13007,7 +13004,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>225</v>
       </c>
@@ -13159,7 +13156,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>225</v>
       </c>
@@ -13311,7 +13308,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>225</v>
       </c>
@@ -13463,7 +13460,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>225</v>
       </c>
@@ -13609,7 +13606,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>232</v>
       </c>
@@ -13761,7 +13758,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>232</v>
       </c>
@@ -13913,7 +13910,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>232</v>
       </c>
@@ -14065,7 +14062,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>237</v>
       </c>
@@ -14217,7 +14214,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>240</v>
       </c>
@@ -14369,7 +14366,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>240</v>
       </c>
@@ -14521,7 +14518,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>240</v>
       </c>
@@ -14673,7 +14670,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>240</v>
       </c>
@@ -14825,7 +14822,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>247</v>
       </c>
@@ -14977,7 +14974,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>250</v>
       </c>
@@ -15129,7 +15126,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>250</v>
       </c>
@@ -15281,7 +15278,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>254</v>
       </c>
@@ -15433,7 +15430,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>257</v>
       </c>
@@ -15585,7 +15582,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>260</v>
       </c>
@@ -15737,7 +15734,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>260</v>
       </c>
@@ -15889,7 +15886,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>260</v>
       </c>
@@ -16041,7 +16038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>260</v>
       </c>
@@ -16193,7 +16190,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="96" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>266</v>
       </c>
@@ -16345,7 +16342,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>266</v>
       </c>
@@ -16497,7 +16494,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="98" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>270</v>
       </c>
@@ -16649,7 +16646,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="99" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>273</v>
       </c>
@@ -16798,7 +16795,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>273</v>
       </c>
@@ -16947,7 +16944,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>277</v>
       </c>
@@ -17099,7 +17096,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>277</v>
       </c>
@@ -17251,7 +17248,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="103" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>277</v>
       </c>
@@ -17403,7 +17400,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="104" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>277</v>
       </c>
@@ -17555,7 +17552,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="105" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>277</v>
       </c>
@@ -17707,7 +17704,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>277</v>
       </c>
@@ -17859,7 +17856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>277</v>
       </c>
@@ -18011,7 +18008,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="108" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>286</v>
       </c>
@@ -18163,7 +18160,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="109" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>289</v>
       </c>
@@ -18315,7 +18312,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="110" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>289</v>
       </c>
@@ -18467,7 +18464,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>293</v>
       </c>
@@ -18619,7 +18616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="112" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>296</v>
       </c>
@@ -18771,7 +18768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>299</v>
       </c>
@@ -18920,7 +18917,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="114" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>299</v>
       </c>
@@ -19072,7 +19069,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>299</v>
       </c>
@@ -19224,7 +19221,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="116" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>304</v>
       </c>
@@ -19376,7 +19373,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="117" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>307</v>
       </c>
@@ -19528,7 +19525,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="118" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>310</v>
       </c>
@@ -19680,7 +19677,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="119" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>313</v>
       </c>
@@ -19832,7 +19829,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>316</v>
       </c>
@@ -19984,7 +19981,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>316</v>
       </c>
@@ -20136,7 +20133,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>320</v>
       </c>
@@ -20285,7 +20282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="123" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>323</v>
       </c>
@@ -20437,7 +20434,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>323</v>
       </c>
@@ -20589,7 +20586,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="125" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>327</v>
       </c>
@@ -20741,7 +20738,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>330</v>
       </c>
@@ -20893,7 +20890,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="127" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>333</v>
       </c>
@@ -21045,7 +21042,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>333</v>
       </c>
@@ -21197,7 +21194,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>337</v>
       </c>
@@ -21349,7 +21346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="130" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>340</v>
       </c>
@@ -21501,7 +21498,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="131" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>343</v>
       </c>
@@ -21653,12 +21650,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="132" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>349</v>
+      </c>
+      <c r="B132" t="s">
         <v>346</v>
-      </c>
-      <c r="B132" t="s">
-        <v>347</v>
       </c>
       <c r="C132" s="1">
         <v>5.75</v>
@@ -21670,7 +21667,7 @@
         <v>38645</v>
       </c>
       <c r="F132" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H132" t="s">
         <v>53</v>
@@ -21805,12 +21802,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="133" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>349</v>
+      </c>
+      <c r="B133" t="s">
         <v>346</v>
-      </c>
-      <c r="B133" t="s">
-        <v>347</v>
       </c>
       <c r="C133" s="1">
         <v>5.75</v>
@@ -21822,7 +21819,7 @@
         <v>38645</v>
       </c>
       <c r="F133" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H133" t="s">
         <v>53</v>
@@ -21957,12 +21954,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="134" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>349</v>
+      </c>
+      <c r="B134" t="s">
         <v>350</v>
-      </c>
-      <c r="B134" t="s">
-        <v>351</v>
       </c>
       <c r="C134" s="1">
         <v>7.75</v>
@@ -21974,7 +21971,7 @@
         <v>36350</v>
       </c>
       <c r="F134" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H134" t="s">
         <v>53</v>
@@ -22109,12 +22106,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="135" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
+        <v>349</v>
+      </c>
+      <c r="B135" t="s">
         <v>350</v>
-      </c>
-      <c r="B135" t="s">
-        <v>351</v>
       </c>
       <c r="C135" s="1">
         <v>7.75</v>
@@ -22126,7 +22123,7 @@
         <v>36517</v>
       </c>
       <c r="F135" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H135" t="s">
         <v>53</v>
@@ -22261,12 +22258,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="136" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>349</v>
+      </c>
+      <c r="B136" t="s">
         <v>350</v>
-      </c>
-      <c r="B136" t="s">
-        <v>351</v>
       </c>
       <c r="C136" s="1">
         <v>7.75</v>
@@ -22278,7 +22275,7 @@
         <v>36350</v>
       </c>
       <c r="F136" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H136" t="s">
         <v>53</v>
@@ -22413,12 +22410,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="137" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>349</v>
+      </c>
+      <c r="B137" t="s">
         <v>350</v>
-      </c>
-      <c r="B137" t="s">
-        <v>351</v>
       </c>
       <c r="C137" s="1">
         <v>7.75</v>
@@ -22430,7 +22427,7 @@
         <v>36350</v>
       </c>
       <c r="F137" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H137" t="s">
         <v>53</v>
@@ -22565,12 +22562,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="138" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>349</v>
+      </c>
+      <c r="B138" t="s">
         <v>350</v>
-      </c>
-      <c r="B138" t="s">
-        <v>351</v>
       </c>
       <c r="C138" s="1">
         <v>7.75</v>
@@ -22582,7 +22579,7 @@
         <v>36350</v>
       </c>
       <c r="F138" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H138" t="s">
         <v>53</v>
@@ -22717,12 +22714,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="139" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>349</v>
+      </c>
+      <c r="B139" t="s">
         <v>350</v>
-      </c>
-      <c r="B139" t="s">
-        <v>351</v>
       </c>
       <c r="C139" s="1">
         <v>2.875</v>
@@ -22734,7 +22731,7 @@
         <v>41967</v>
       </c>
       <c r="F139" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H139" t="s">
         <v>53</v>
@@ -22869,12 +22866,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="140" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>357</v>
+      </c>
+      <c r="B140" t="s">
         <v>358</v>
-      </c>
-      <c r="B140" t="s">
-        <v>359</v>
       </c>
       <c r="C140" s="1">
         <v>9.875</v>
@@ -22886,7 +22883,7 @@
         <v>31470</v>
       </c>
       <c r="F140" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H140" t="s">
         <v>53</v>
@@ -23021,12 +23018,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="141" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>360</v>
+      </c>
+      <c r="B141" t="s">
         <v>361</v>
-      </c>
-      <c r="B141" t="s">
-        <v>362</v>
       </c>
       <c r="C141" s="1">
         <v>5.125</v>
@@ -23038,7 +23035,7 @@
         <v>36178</v>
       </c>
       <c r="F141" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H141" t="s">
         <v>53</v>
@@ -23173,12 +23170,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="142" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>360</v>
+      </c>
+      <c r="B142" t="s">
         <v>361</v>
-      </c>
-      <c r="B142" t="s">
-        <v>362</v>
       </c>
       <c r="C142" s="1">
         <v>5.125</v>
@@ -23190,7 +23187,7 @@
         <v>36220</v>
       </c>
       <c r="F142" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H142" t="s">
         <v>53</v>
@@ -23325,12 +23322,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>360</v>
+      </c>
+      <c r="B143" t="s">
         <v>361</v>
-      </c>
-      <c r="B143" t="s">
-        <v>362</v>
       </c>
       <c r="C143" s="1">
         <v>5.125</v>
@@ -23342,7 +23339,7 @@
         <v>36236</v>
       </c>
       <c r="F143" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H143" t="s">
         <v>53</v>
@@ -23477,12 +23474,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>360</v>
+      </c>
+      <c r="B144" t="s">
         <v>361</v>
-      </c>
-      <c r="B144" t="s">
-        <v>362</v>
       </c>
       <c r="C144" s="1">
         <v>4</v>
@@ -23494,7 +23491,7 @@
         <v>36777</v>
       </c>
       <c r="F144" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H144" t="s">
         <v>53</v>
@@ -23629,12 +23626,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="145" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>360</v>
+      </c>
+      <c r="B145" t="s">
         <v>361</v>
-      </c>
-      <c r="B145" t="s">
-        <v>362</v>
       </c>
       <c r="C145" s="1">
         <v>6.625</v>
@@ -23646,7 +23643,7 @@
         <v>36811</v>
       </c>
       <c r="F145" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H145" t="s">
         <v>53</v>
@@ -23781,12 +23778,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="146" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>360</v>
+      </c>
+      <c r="B146" t="s">
         <v>361</v>
-      </c>
-      <c r="B146" t="s">
-        <v>362</v>
       </c>
       <c r="C146" s="1">
         <v>6</v>
@@ -23798,7 +23795,7 @@
         <v>37055</v>
       </c>
       <c r="F146" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H146" t="s">
         <v>53</v>
@@ -23933,12 +23930,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="147" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>360</v>
+      </c>
+      <c r="B147" t="s">
         <v>361</v>
-      </c>
-      <c r="B147" t="s">
-        <v>362</v>
       </c>
       <c r="C147" s="1">
         <v>3.3220000000000001</v>
@@ -23950,7 +23947,7 @@
         <v>37603</v>
       </c>
       <c r="F147" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H147" t="s">
         <v>53</v>
@@ -24085,12 +24082,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="148" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>360</v>
+      </c>
+      <c r="B148" t="s">
         <v>361</v>
-      </c>
-      <c r="B148" t="s">
-        <v>362</v>
       </c>
       <c r="C148" s="1">
         <v>5.5</v>
@@ -24102,7 +24099,7 @@
         <v>37603</v>
       </c>
       <c r="F148" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H148" t="s">
         <v>53</v>
@@ -24237,12 +24234,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="149" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>360</v>
+      </c>
+      <c r="B149" t="s">
         <v>361</v>
-      </c>
-      <c r="B149" t="s">
-        <v>362</v>
       </c>
       <c r="C149" s="1">
         <v>6</v>
@@ -24254,7 +24251,7 @@
         <v>37055</v>
       </c>
       <c r="F149" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H149" t="s">
         <v>53</v>
@@ -24389,12 +24386,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="150" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>360</v>
+      </c>
+      <c r="B150" t="s">
         <v>361</v>
-      </c>
-      <c r="B150" t="s">
-        <v>362</v>
       </c>
       <c r="C150" s="1">
         <v>5</v>
@@ -24406,7 +24403,7 @@
         <v>39373</v>
       </c>
       <c r="F150" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H150" t="s">
         <v>53</v>
@@ -24541,12 +24538,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="151" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
+        <v>360</v>
+      </c>
+      <c r="B151" t="s">
         <v>361</v>
-      </c>
-      <c r="B151" t="s">
-        <v>362</v>
       </c>
       <c r="C151" s="1">
         <v>5</v>
@@ -24558,7 +24555,7 @@
         <v>39735</v>
       </c>
       <c r="F151" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H151" t="s">
         <v>53</v>
@@ -24693,12 +24690,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="152" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>360</v>
+      </c>
+      <c r="B152" t="s">
         <v>361</v>
-      </c>
-      <c r="B152" t="s">
-        <v>362</v>
       </c>
       <c r="C152" s="1">
         <v>5</v>
@@ -24710,7 +24707,7 @@
         <v>39868</v>
       </c>
       <c r="F152" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H152" t="s">
         <v>53</v>
@@ -24845,12 +24842,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="153" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>360</v>
+      </c>
+      <c r="B153" t="s">
         <v>361</v>
-      </c>
-      <c r="B153" t="s">
-        <v>362</v>
       </c>
       <c r="C153" s="1">
         <v>6.125</v>
@@ -24862,7 +24859,7 @@
         <v>39868</v>
       </c>
       <c r="F153" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H153" t="s">
         <v>53</v>
@@ -24904,105 +24901,105 @@
         <v>1</v>
       </c>
       <c r="U153" t="s">
+        <v>375</v>
+      </c>
+      <c r="V153" t="s">
+        <v>19</v>
+      </c>
+      <c r="W153" t="s">
         <v>376</v>
       </c>
-      <c r="V153" t="s">
-        <v>19</v>
-      </c>
-      <c r="W153" t="s">
+      <c r="X153" t="s">
+        <v>376</v>
+      </c>
+      <c r="Y153" t="s">
         <v>377</v>
       </c>
-      <c r="X153" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y153" t="s">
+      <c r="Z153" t="s">
         <v>378</v>
       </c>
-      <c r="Z153" t="s">
+      <c r="AA153" t="s">
         <v>379</v>
       </c>
-      <c r="AA153" t="s">
+      <c r="AB153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF153" t="s">
         <v>380</v>
       </c>
-      <c r="AB153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF153" t="s">
+      <c r="AG153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS153" t="s">
+        <v>376</v>
+      </c>
+      <c r="AT153" t="s">
         <v>381</v>
       </c>
-      <c r="AG153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AM153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AN153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AO153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AP153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AQ153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AR153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AS153" t="s">
-        <v>377</v>
-      </c>
-      <c r="AT153" t="s">
+      <c r="AU153" t="s">
         <v>382</v>
       </c>
-      <c r="AU153" t="s">
+      <c r="AV153" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW153" t="s">
         <v>383</v>
       </c>
-      <c r="AV153" t="s">
-        <v>19</v>
-      </c>
-      <c r="AW153" t="s">
+      <c r="AX153" t="s">
         <v>384</v>
       </c>
-      <c r="AX153" t="s">
+      <c r="AY153" t="s">
         <v>385</v>
       </c>
-      <c r="AY153" t="s">
+    </row>
+    <row r="154" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="154" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
+      <c r="B154" t="s">
         <v>387</v>
-      </c>
-      <c r="B154" t="s">
-        <v>388</v>
       </c>
       <c r="C154" s="1">
         <v>3.5</v>
@@ -25014,7 +25011,7 @@
         <v>42124</v>
       </c>
       <c r="F154" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H154" t="s">
         <v>53</v>
@@ -25149,12 +25146,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
+        <v>389</v>
+      </c>
+      <c r="B155" t="s">
         <v>390</v>
-      </c>
-      <c r="B155" t="s">
-        <v>391</v>
       </c>
       <c r="C155" s="1">
         <v>7.75</v>
@@ -25166,7 +25163,7 @@
         <v>40290</v>
       </c>
       <c r="F155" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H155" t="s">
         <v>53</v>
@@ -25301,12 +25298,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="156" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>392</v>
+      </c>
+      <c r="B156" t="s">
         <v>393</v>
-      </c>
-      <c r="B156" t="s">
-        <v>394</v>
       </c>
       <c r="C156" s="1">
         <v>4.375</v>
@@ -25318,7 +25315,7 @@
         <v>41897</v>
       </c>
       <c r="F156" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H156" t="s">
         <v>53</v>
@@ -25453,12 +25450,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="157" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
+        <v>395</v>
+      </c>
+      <c r="B157" t="s">
         <v>396</v>
-      </c>
-      <c r="B157" t="s">
-        <v>397</v>
       </c>
       <c r="C157" s="1">
         <v>11</v>
@@ -25470,7 +25467,7 @@
         <v>31462</v>
       </c>
       <c r="F157" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H157" t="s">
         <v>53</v>
@@ -25605,12 +25602,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="158" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>398</v>
+      </c>
+      <c r="B158" t="s">
         <v>399</v>
-      </c>
-      <c r="B158" t="s">
-        <v>400</v>
       </c>
       <c r="C158" s="1">
         <v>6.5</v>
@@ -25622,7 +25619,7 @@
         <v>40140</v>
       </c>
       <c r="F158" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H158" t="s">
         <v>53</v>
@@ -25757,12 +25754,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>401</v>
+      </c>
+      <c r="B159" t="s">
         <v>402</v>
-      </c>
-      <c r="B159" t="s">
-        <v>403</v>
       </c>
       <c r="C159" s="1">
         <v>5.25</v>
@@ -25774,7 +25771,7 @@
         <v>37551</v>
       </c>
       <c r="F159" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H159" t="s">
         <v>53</v>
@@ -25909,12 +25906,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="160" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>401</v>
+      </c>
+      <c r="B160" t="s">
         <v>402</v>
-      </c>
-      <c r="B160" t="s">
-        <v>403</v>
       </c>
       <c r="C160" s="1">
         <v>5.625</v>
@@ -25926,7 +25923,7 @@
         <v>37610</v>
       </c>
       <c r="F160" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H160" t="s">
         <v>53</v>
@@ -26061,12 +26058,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="161" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
+        <v>401</v>
+      </c>
+      <c r="B161" t="s">
         <v>402</v>
-      </c>
-      <c r="B161" t="s">
-        <v>403</v>
       </c>
       <c r="C161" s="1">
         <v>5.375</v>
@@ -26078,7 +26075,7 @@
         <v>37755</v>
       </c>
       <c r="F161" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H161" t="s">
         <v>53</v>
@@ -26213,12 +26210,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="162" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
+        <v>401</v>
+      </c>
+      <c r="B162" t="s">
         <v>402</v>
-      </c>
-      <c r="B162" t="s">
-        <v>403</v>
       </c>
       <c r="C162" s="1">
         <v>5.625</v>
@@ -26230,7 +26227,7 @@
         <v>37610</v>
       </c>
       <c r="F162" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H162" t="s">
         <v>53</v>
@@ -26365,12 +26362,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>401</v>
+      </c>
+      <c r="B163" t="s">
         <v>402</v>
-      </c>
-      <c r="B163" t="s">
-        <v>403</v>
       </c>
       <c r="C163" s="1">
         <v>1.5865</v>
@@ -26382,7 +26379,7 @@
         <v>38945</v>
       </c>
       <c r="F163" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H163" t="s">
         <v>53</v>
@@ -26517,12 +26514,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="164" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>401</v>
+      </c>
+      <c r="B164" t="s">
         <v>402</v>
-      </c>
-      <c r="B164" t="s">
-        <v>403</v>
       </c>
       <c r="C164" s="1">
         <v>6.125</v>
@@ -26534,7 +26531,7 @@
         <v>39811</v>
       </c>
       <c r="F164" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H164" t="s">
         <v>53</v>
@@ -26669,12 +26666,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="165" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
+        <v>401</v>
+      </c>
+      <c r="B165" t="s">
         <v>402</v>
-      </c>
-      <c r="B165" t="s">
-        <v>403</v>
       </c>
       <c r="C165" s="1">
         <v>6.125</v>
@@ -26686,7 +26683,7 @@
         <v>39829</v>
       </c>
       <c r="F165" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H165" t="s">
         <v>53</v>
@@ -26821,12 +26818,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="166" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
+        <v>401</v>
+      </c>
+      <c r="B166" t="s">
         <v>402</v>
-      </c>
-      <c r="B166" t="s">
-        <v>403</v>
       </c>
       <c r="C166" s="1">
         <v>6.125</v>
@@ -26838,7 +26835,7 @@
         <v>39862</v>
       </c>
       <c r="F166" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H166" t="s">
         <v>53</v>
@@ -26973,12 +26970,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="167" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
+        <v>401</v>
+      </c>
+      <c r="B167" t="s">
         <v>402</v>
-      </c>
-      <c r="B167" t="s">
-        <v>403</v>
       </c>
       <c r="C167" s="1">
         <v>5.75</v>
@@ -26990,7 +26987,7 @@
         <v>39897</v>
       </c>
       <c r="F167" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H167" t="s">
         <v>53</v>
@@ -27125,12 +27122,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
+        <v>401</v>
+      </c>
+      <c r="B168" t="s">
         <v>402</v>
-      </c>
-      <c r="B168" t="s">
-        <v>403</v>
       </c>
       <c r="C168" s="1">
         <v>5.75</v>
@@ -27142,7 +27139,7 @@
         <v>39976</v>
       </c>
       <c r="F168" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H168" t="s">
         <v>53</v>
@@ -27277,12 +27274,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="169" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
+        <v>401</v>
+      </c>
+      <c r="B169" t="s">
         <v>402</v>
-      </c>
-      <c r="B169" t="s">
-        <v>403</v>
       </c>
       <c r="C169" s="1">
         <v>6.125</v>
@@ -27294,7 +27291,7 @@
         <v>39993</v>
       </c>
       <c r="F169" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H169" t="s">
         <v>53</v>
@@ -27429,12 +27426,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="170" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
+        <v>414</v>
+      </c>
+      <c r="B170" t="s">
         <v>415</v>
-      </c>
-      <c r="B170" t="s">
-        <v>416</v>
       </c>
       <c r="C170" s="1">
         <v>2.544</v>
@@ -27446,7 +27443,7 @@
         <v>43852</v>
       </c>
       <c r="F170" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H170" t="s">
         <v>53</v>
@@ -27581,12 +27578,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="171" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>417</v>
+      </c>
+      <c r="B171" t="s">
         <v>418</v>
-      </c>
-      <c r="B171" t="s">
-        <v>419</v>
       </c>
       <c r="C171" s="1">
         <v>4.75</v>
@@ -27598,7 +27595,7 @@
         <v>37650</v>
       </c>
       <c r="F171" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H171" t="s">
         <v>53</v>
@@ -27733,12 +27730,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="172" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>420</v>
+      </c>
+      <c r="B172" t="s">
         <v>421</v>
-      </c>
-      <c r="B172" t="s">
-        <v>422</v>
       </c>
       <c r="C172" s="1">
         <v>8.125</v>
@@ -27750,7 +27747,7 @@
         <v>38085</v>
       </c>
       <c r="F172" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H172" t="s">
         <v>53</v>
@@ -27885,12 +27882,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="173" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>423</v>
+      </c>
+      <c r="B173" t="s">
         <v>424</v>
-      </c>
-      <c r="B173" t="s">
-        <v>425</v>
       </c>
       <c r="C173" s="1">
         <v>7.125</v>
@@ -27902,7 +27899,7 @@
         <v>40129</v>
       </c>
       <c r="F173" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H173" t="s">
         <v>53</v>
@@ -28037,12 +28034,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>423</v>
+      </c>
+      <c r="B174" t="s">
         <v>424</v>
-      </c>
-      <c r="B174" t="s">
-        <v>425</v>
       </c>
       <c r="C174" s="1">
         <v>4.25</v>
@@ -28054,7 +28051,7 @@
         <v>41430</v>
       </c>
       <c r="F174" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H174" t="s">
         <v>53</v>
@@ -28189,12 +28186,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>423</v>
+      </c>
+      <c r="B175" t="s">
         <v>424</v>
-      </c>
-      <c r="B175" t="s">
-        <v>425</v>
       </c>
       <c r="C175" s="1">
         <v>4.875</v>
@@ -28206,7 +28203,7 @@
         <v>42517</v>
       </c>
       <c r="F175" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H175" t="s">
         <v>53</v>
@@ -28341,12 +28338,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="176" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>428</v>
+      </c>
+      <c r="B176" t="s">
         <v>429</v>
-      </c>
-      <c r="B176" t="s">
-        <v>430</v>
       </c>
       <c r="C176" s="1">
         <v>6</v>
@@ -28358,7 +28355,7 @@
         <v>37243</v>
       </c>
       <c r="F176" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H176" t="s">
         <v>53</v>
@@ -28493,12 +28490,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="177" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>428</v>
+      </c>
+      <c r="B177" t="s">
         <v>429</v>
-      </c>
-      <c r="B177" t="s">
-        <v>430</v>
       </c>
       <c r="C177" s="1">
         <v>4.625</v>
@@ -28510,7 +28507,7 @@
         <v>40885</v>
       </c>
       <c r="F177" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H177" t="s">
         <v>53</v>
@@ -28645,12 +28642,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="178" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>432</v>
+      </c>
+      <c r="B178" t="s">
         <v>433</v>
-      </c>
-      <c r="B178" t="s">
-        <v>434</v>
       </c>
       <c r="C178" s="1">
         <v>6</v>
@@ -28662,7 +28659,7 @@
         <v>41191</v>
       </c>
       <c r="F178" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H178" t="s">
         <v>53</v>
@@ -28797,12 +28794,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="179" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>435</v>
+      </c>
+      <c r="B179" t="s">
         <v>436</v>
-      </c>
-      <c r="B179" t="s">
-        <v>437</v>
       </c>
       <c r="C179" s="1">
         <v>6</v>
@@ -28814,7 +28811,7 @@
         <v>39176</v>
       </c>
       <c r="F179" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H179" t="s">
         <v>53</v>
@@ -28949,12 +28946,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="180" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>438</v>
+      </c>
+      <c r="B180" t="s">
         <v>439</v>
-      </c>
-      <c r="B180" t="s">
-        <v>440</v>
       </c>
       <c r="C180" s="1">
         <v>0</v>
@@ -28966,7 +28963,7 @@
         <v>42164</v>
       </c>
       <c r="F180" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H180" t="s">
         <v>53</v>
@@ -29098,12 +29095,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>438</v>
+      </c>
+      <c r="B181" t="s">
         <v>439</v>
-      </c>
-      <c r="B181" t="s">
-        <v>440</v>
       </c>
       <c r="C181" s="1">
         <v>0</v>
@@ -29115,7 +29112,7 @@
         <v>42164</v>
       </c>
       <c r="F181" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H181" t="s">
         <v>53</v>

</xml_diff>